<commit_message>
cambios en txt y exel
</commit_message>
<xml_diff>
--- a/resumen archivo excel.xlsx
+++ b/resumen archivo excel.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cristian.ciambrignon\Desktop\working\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -69,7 +74,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -331,12 +336,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>